<commit_message>
Feature: Additional dynamic pandapipes simulation
</commit_message>
<xml_diff>
--- a/uesgraphs/data/uesgraphs_parameters_template_pp.xlsx
+++ b/uesgraphs/data/uesgraphs_parameters_template_pp.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <t xml:space="preserve">uesgraphs Parameter Template</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t xml:space="preserve">timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dynamic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode for dynamic or static simulation must be set either to „dynamic“ or to „static“</t>
   </si>
   <si>
     <t xml:space="preserve">save_params_to_csv</t>
@@ -1189,6 +1198,7 @@
         <v>40</v>
       </c>
       <c r="B4" s="14" t="n">
+        <f aca="false">3600*24*365</f>
         <v>31536000</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1211,34 +1221,47 @@
       <c r="D5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1292,44 +1315,44 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2" s="14" t="n">
         <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" s="14" t="n">
         <v>4180</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B4" s="18" t="n">
         <v>323.15</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E4" s="15"/>
     </row>
@@ -1404,67 +1427,67 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B2" s="14" t="n">
         <v>800000</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B3" s="18" t="n">
         <v>600000</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B4" s="14" t="n">
         <f aca="false">B2-B3</f>
         <v>200000</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B5" s="14" t="n">
         <v>353.15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B6" s="18" t="n">
         <v>323.15</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E6" s="15"/>
     </row>
@@ -1523,63 +1546,63 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B2" s="19" t="n">
         <v>0.04</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B3" s="19" t="n">
         <v>0.03</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B4" s="14" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B5" s="14" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>5</v>
@@ -1588,7 +1611,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1630,118 +1653,118 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1749,37 +1772,37 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F16" s="5"/>
     </row>

</xml_diff>

<commit_message>
Fix and Feature: Start time is now available for more than default 0 in pandapipes simulations
</commit_message>
<xml_diff>
--- a/uesgraphs/data/uesgraphs_parameters_template_pp.xlsx
+++ b/uesgraphs/data/uesgraphs_parameters_template_pp.xlsx
@@ -1140,7 +1140,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1184,7 +1184,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="14" t="n">
-        <v>0</v>
+        <v>3600</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>38</v>
@@ -1198,8 +1198,8 @@
         <v>40</v>
       </c>
       <c r="B4" s="14" t="n">
-        <f aca="false">3600*24*365</f>
-        <v>31536000</v>
+        <f aca="false">3600*24</f>
+        <v>86400</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>38</v>

</xml_diff>